<commit_message>
Correct reported column in coercion warnings
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/geometry.xlsx
+++ b/tests/testthat/sheets/geometry.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14980" yWindow="460" windowWidth="11380" windowHeight="11000" tabRatio="500"/>
+    <workbookView xWindow="14980" yWindow="460" windowWidth="11380" windowHeight="11000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="warning_position" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>var1</t>
   </si>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t>ii</t>
+  </si>
+  <si>
+    <t>wtf</t>
   </si>
 </sst>
 </file>
@@ -379,7 +383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -432,4 +436,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Report problematic cells in A1 / R1C1 notation; fixes #230
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/geometry.xlsx
+++ b/tests/testthat/sheets/geometry.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14980" yWindow="460" windowWidth="11380" windowHeight="11000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14980" yWindow="460" windowWidth="11380" windowHeight="11000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="warning_position" sheetId="2" r:id="rId2"/>
+    <sheet name="warning_B6" sheetId="2" r:id="rId2"/>
+    <sheet name="warning_AT6" sheetId="3" r:id="rId3"/>
+    <sheet name="warning_AKE6" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>var1</t>
   </si>
@@ -442,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="AKC1" workbookViewId="0">
+      <selection activeCell="AKD2" sqref="AKD2:AKF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,4 +473,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="AT3:AT6"/>
+  <sheetViews>
+    <sheetView topLeftCell="AKC1" workbookViewId="0">
+      <selection activeCell="AKD2" sqref="AKD2:AKF7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="5" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT5">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="6" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="AKE3:AKE6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AS2" sqref="AS2:AU9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="967:967" x14ac:dyDescent="0.2">
+      <c r="AKE3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="967:967" x14ac:dyDescent="0.2">
+      <c r="AKE4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="5" spans="967:967" x14ac:dyDescent="0.2">
+      <c r="AKE5">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="6" spans="967:967" x14ac:dyDescent="0.2">
+      <c r="AKE6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Report problematic cells in A1 notation (#336)
* Correct reported column in coercion warnings

* Utility functions to make A1 refs

* Report problematic cells in A1 / R1C1 notation; fixes #230

* Rename to cellPosition() and do `+ 1` in there

* Format switches() consistently
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/geometry.xlsx
+++ b/tests/testthat/sheets/geometry.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14980" yWindow="460" windowWidth="11380" windowHeight="11000" tabRatio="500"/>
+    <workbookView xWindow="14980" yWindow="460" windowWidth="11380" windowHeight="11000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="warning_B6" sheetId="2" r:id="rId2"/>
+    <sheet name="warning_AT6" sheetId="3" r:id="rId3"/>
+    <sheet name="warning_AKE6" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>var1</t>
   </si>
@@ -63,6 +66,9 @@
   </si>
   <si>
     <t>ii</t>
+  </si>
+  <si>
+    <t>wtf</t>
   </si>
 </sst>
 </file>
@@ -379,7 +385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -432,4 +438,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B6"/>
+  <sheetViews>
+    <sheetView topLeftCell="AKC1" workbookViewId="0">
+      <selection activeCell="AKD2" sqref="AKD2:AKF7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="AT3:AT6"/>
+  <sheetViews>
+    <sheetView topLeftCell="AKC1" workbookViewId="0">
+      <selection activeCell="AKD2" sqref="AKD2:AKF7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="5" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT5">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="6" spans="46:46" x14ac:dyDescent="0.2">
+      <c r="AT6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="AKE3:AKE6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AS2" sqref="AS2:AU9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="967:967" x14ac:dyDescent="0.2">
+      <c r="AKE3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="967:967" x14ac:dyDescent="0.2">
+      <c r="AKE4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="5" spans="967:967" x14ac:dyDescent="0.2">
+      <c r="AKE5">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="6" spans="967:967" x14ac:dyDescent="0.2">
+      <c r="AKE6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>